<commit_message>
Re-ran program query after series finished
</commit_message>
<xml_diff>
--- a/foodfight_program_query.xlsx
+++ b/foodfight_program_query.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results" sheetId="1" r:id="R1d4f1b205f5d4e5e"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results" sheetId="1" r:id="R20f9dedff78e4ba1"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -403,16 +403,42 @@
         <x:v>18</x:v>
       </x:c>
       <x:c s="3">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c s="3">
-        <x:v>0.0000</x:v>
-      </x:c>
-      <x:c s="1" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c s="3">
-        <x:v>51</x:v>
+        <x:v>55</x:v>
+      </x:c>
+      <x:c s="3">
+        <x:v>1.0000</x:v>
+      </x:c>
+      <x:c s="1" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c s="3">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c s="1" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c s="1" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c s="2">
+        <x:v>45459</x:v>
+      </x:c>
+      <x:c s="1" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c s="3">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c s="3">
+        <x:v>1.0000</x:v>
+      </x:c>
+      <x:c s="1" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c s="3">
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row>

</xml_diff>